<commit_message>
Input Output Completed bug fixed
</commit_message>
<xml_diff>
--- a/src/main/resources/Table.xlsx
+++ b/src/main/resources/Table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>CargoId</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>comment4</t>
+  </si>
+  <si>
+    <t>comment5</t>
   </si>
 </sst>
 </file>
@@ -390,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,6 +531,32 @@
         <v>13</v>
       </c>
     </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2">
+        <v>5</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="2">
+        <v>101</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
2d array to images
</commit_message>
<xml_diff>
--- a/src/main/resources/Table.xlsx
+++ b/src/main/resources/Table.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aleksandr Sergijenko\IdeaProjects\LogisticProject\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aserg\IdeaProjects\LogisticProjectFix\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9252ECD-ADA3-490E-9347-B4B6DE36DE72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -74,7 +75,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -115,7 +116,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -392,11 +393,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,7 +552,7 @@
         <v>10</v>
       </c>
       <c r="G6" s="2">
-        <v>101</v>
+        <v>5</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>14</v>

</xml_diff>